<commit_message>
Doku + kleine Verbesserungen + Add Photographer hinzugeüfgt
</commit_message>
<xml_diff>
--- a/Notenrechner Codereview SWE 2.xlsx
+++ b/Notenrechner Codereview SWE 2.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAC67D6-6091-40E1-9E3E-03AB0CEC0639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18315BA-D532-484F-9081-6BA900CC3D45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1133,8 +1133,8 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="117" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1286,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
@@ -1297,7 +1297,9 @@
       <c r="A17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="1"/>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
@@ -1307,7 +1309,9 @@
       <c r="A18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
       <c r="C18" s="7">
         <v>1</v>
       </c>
@@ -1325,7 +1329,9 @@
       <c r="A21" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
       <c r="C21" s="7">
         <v>1</v>
       </c>
@@ -1335,7 +1341,9 @@
       <c r="A22" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
       <c r="C22" s="7">
         <v>1</v>
       </c>
@@ -1353,7 +1361,9 @@
       <c r="A25" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
       <c r="C25" s="7">
         <v>2</v>
       </c>
@@ -1363,7 +1373,9 @@
       <c r="A26" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="1"/>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
       <c r="C26" s="7">
         <v>1</v>
       </c>
@@ -1373,7 +1385,9 @@
       <c r="A27" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
       <c r="C27" s="7">
         <v>1</v>
       </c>
@@ -1417,7 +1431,7 @@
       </c>
       <c r="B33" s="5">
         <f>SUM(B6:B27)-SUM(B30:B32)</f>
-        <v>11.5</v>
+        <v>13</v>
       </c>
       <c r="C33" s="5">
         <f>SUM(C6:C27)</f>

</xml_diff>